<commit_message>
last push before going oop
</commit_message>
<xml_diff>
--- a/riskmanagement_project/BLACK_SHOELS_RESULTS/simulated_stock_prices.xlsx
+++ b/riskmanagement_project/BLACK_SHOELS_RESULTS/simulated_stock_prices.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40.37724845450484</v>
+        <v>49.46212935676843</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40.27269048522573</v>
+        <v>49.33602558098684</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>40.76948198008294</v>
+        <v>49.94662382203796</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41.96082453768333</v>
+        <v>51.40819847409598</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>41.77639283427928</v>
+        <v>51.18429634055894</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>41.59278467407381</v>
+        <v>50.96138519705672</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>42.85366139024801</v>
+        <v>52.50837614737682</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>43.480575817052</v>
+        <v>53.27866919244317</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>43.09737703881376</v>
+        <v>52.81123799998915</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>43.54241946033192</v>
+        <v>53.35873116925643</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43.16361590444845</v>
+        <v>52.89665181037189</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>42.78623826876611</v>
+        <v>52.43628280325093</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>42.98319547641006</v>
+        <v>52.67977582013763</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>41.45762008455145</v>
+        <v>50.81208479764181</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>40.12878406421529</v>
+        <v>49.18538495699213</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>39.70542040967335</v>
+        <v>48.66842598591379</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>38.95343926071564</v>
+        <v>47.7486104684644</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>39.18624719488259</v>
+        <v>48.03591092007464</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>38.5203190852028</v>
+        <v>47.22148718216683</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>37.50656196925878</v>
+        <v>45.9805824775968</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>38.56071939002329</v>
+        <v>47.27480728948368</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>38.39731054047639</v>
+        <v>47.07635979114276</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>38.44711445505142</v>
+        <v>47.13931260866798</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>37.42648095466292</v>
+        <v>45.88977375508578</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>37.0441594083638</v>
+        <v>45.42282011073564</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>37.12263912949511</v>
+        <v>45.52087704596488</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>36.32460490718369</v>
+        <v>44.54409134900789</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>36.58416228017145</v>
+        <v>44.86418133387139</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>36.17196900790002</v>
+        <v>44.36047727624057</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>35.97384161612359</v>
+        <v>44.11926876524473</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>35.56780698785363</v>
+        <v>43.62304766969089</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>36.835636591809</v>
+        <v>45.17982271105376</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>36.8269808893217</v>
+        <v>45.17101888191685</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>36.09888431231411</v>
+        <v>44.27973135855528</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>36.66514811796603</v>
+        <v>44.97612850137143</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>35.82962084361885</v>
+        <v>43.95297390773155</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>35.9720469885351</v>
+        <v>44.1294619620521</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>34.66491028131651</v>
+        <v>42.52761116391168</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>33.80631608432192</v>
+        <v>41.47593481417574</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>33.93300173341115</v>
+        <v>41.63303219467908</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>34.41057101404713</v>
+        <v>42.22066505917076</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>34.5228848943926</v>
+        <v>42.36017039404746</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>34.4482070634636</v>
+        <v>42.27023562123649</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>34.25342948785102</v>
+        <v>42.0329172932786</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>33.31025527154303</v>
+        <v>40.87717381264002</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>32.86083762652012</v>
+        <v>40.32728252110365</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>32.57667080572294</v>
+        <v>39.98015330620286</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>33.2346899756399</v>
+        <v>40.78935287917128</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>33.45188202081569</v>
+        <v>41.05756294875189</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>32.35633361091016</v>
+        <v>39.71452230227865</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>32.55576487534513</v>
+        <v>39.96090998109428</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>32.32035296126909</v>
+        <v>39.67354319905203</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>31.91016449597025</v>
+        <v>39.17160478707117</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>32.28182101091133</v>
+        <v>39.62942526457849</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>32.91762993566107</v>
+        <v>40.41157107632936</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>33.50276533477417</v>
+        <v>41.13156737429249</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>32.97627377919853</v>
+        <v>40.48681483589817</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>32.78479451562818</v>
+        <v>40.25334030966025</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>32.99134256991871</v>
+        <v>40.50856659103023</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>33.6058888458095</v>
+        <v>41.2647958244423</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>33.30361125396634</v>
+        <v>40.89526907510976</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>33.18763200391532</v>
+        <v>40.75448738803336</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>32.5016083221849</v>
+        <v>39.91365038982944</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>31.77575122591904</v>
+        <v>39.02382639236231</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>32.26809004989259</v>
+        <v>39.63005836912316</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>33.10649243916052</v>
+        <v>40.66137399995906</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>33.06213302651354</v>
+        <v>40.6085213188974</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>33.69581560145802</v>
+        <v>41.38850192796388</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>33.92757162895712</v>
+        <v>41.67483969780175</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>33.51712334971661</v>
+        <v>41.17231882461203</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>33.74749701984266</v>
+        <v>41.45697261619378</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>34.74349900145349</v>
+        <v>42.68221985103808</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>34.72068056478363</v>
+        <v>42.65589919147479</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>35.76338272560888</v>
+        <v>43.93866829121426</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>34.03658843308497</v>
+        <v>41.81881771478086</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>34.57008241519479</v>
+        <v>42.47599584642117</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>34.62769298104337</v>
+        <v>42.54848887702006</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>34.43326467590643</v>
+        <v>42.31128456960304</v>
       </c>
     </row>
     <row r="80">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>34.49371982519974</v>
+        <v>42.38727221066272</v>
       </c>
     </row>
     <row r="81">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>33.22278101463573</v>
+        <v>40.82712970612457</v>
       </c>
     </row>
     <row r="82">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>33.08580940223093</v>
+        <v>40.66043832369331</v>
       </c>
     </row>
     <row r="83">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>33.31052219615677</v>
+        <v>40.93823937176331</v>
       </c>
     </row>
     <row r="84">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>34.2546720401242</v>
+        <v>42.10027779099923</v>
       </c>
     </row>
     <row r="85">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>33.92148681814032</v>
+        <v>41.69245366440129</v>
       </c>
     </row>
     <row r="86">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>33.40780697123398</v>
+        <v>41.06274426477556</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>33.09318472714039</v>
+        <v>40.67766297854446</v>
       </c>
     </row>
     <row r="88">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>33.67133560372475</v>
+        <v>41.38997853644605</v>
       </c>
     </row>
     <row r="89">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>33.88186027562737</v>
+        <v>41.65043412817278</v>
       </c>
     </row>
     <row r="90">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>33.54501651878272</v>
+        <v>41.2380122163849</v>
       </c>
     </row>
     <row r="91">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>33.87266071393547</v>
+        <v>41.64246721067363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>